<commit_message>
Eliminar invitacion - estudiante
Se creo la funcion para eliminar la invitacion cuando el dia que sera impartida la tutoria sea igual al dia actual.
</commit_message>
<xml_diff>
--- a/sgtcis/storage/archivos/plantilla_materias.xlsx
+++ b/sgtcis/storage/archivos/plantilla_materias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mejor descripción para la plantilla que se proporciona para el registro de materias
</commit_message>
<xml_diff>
--- a/sgtcis/storage/archivos/plantilla_materias.xlsx
+++ b/sgtcis/storage/archivos/plantilla_materias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="1080" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
   <si>
     <t>nombre</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Economía</t>
+  </si>
+  <si>
+    <t>Séptimo</t>
   </si>
 </sst>
 </file>
@@ -536,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +601,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -766,7 +769,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -906,7 +909,7 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -962,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1060,7 +1063,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>

</xml_diff>